<commit_message>
COVID--19 case data 17 Aug update
</commit_message>
<xml_diff>
--- a/cases/covid-cases-in-hospital-counts-location.xlsx
+++ b/cases/covid-cases-in-hospital-counts-location.xlsx
@@ -427,7 +427,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -64637,7 +64637,7 @@
         <v>44818</v>
       </c>
       <c r="B2">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3">
@@ -76893,7 +76893,7 @@
         <v>44818</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
COVID-19 case data 21 Sept
</commit_message>
<xml_diff>
--- a/cases/covid-cases-in-hospital-counts-location.xlsx
+++ b/cases/covid-cases-in-hospital-counts-location.xlsx
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -947,7 +947,7 @@
         </is>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45">
@@ -973,7 +973,7 @@
         </is>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46">
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47">
@@ -999,7 +999,7 @@
         </is>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -1038,7 +1038,7 @@
         </is>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -1064,7 +1064,7 @@
         </is>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55">
@@ -1103,7 +1103,7 @@
         </is>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
@@ -1116,7 +1116,7 @@
         </is>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
@@ -1129,7 +1129,7 @@
         </is>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59">
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1181,7 +1181,7 @@
         </is>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -1194,7 +1194,7 @@
         </is>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64">
@@ -1220,7 +1220,7 @@
         </is>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65">
@@ -1233,7 +1233,7 @@
         </is>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66">
@@ -1246,7 +1246,7 @@
         </is>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67">
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
@@ -1298,7 +1298,7 @@
         </is>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
@@ -1324,7 +1324,7 @@
         </is>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75">
@@ -1363,7 +1363,7 @@
         </is>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76">
@@ -1376,7 +1376,7 @@
         </is>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77">
@@ -1389,7 +1389,7 @@
         </is>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="79">
@@ -1415,7 +1415,7 @@
         </is>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -1428,7 +1428,7 @@
         </is>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -1441,7 +1441,7 @@
         </is>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -52473,7 +52473,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -52481,7 +52481,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -55633,7 +55633,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -55641,7 +55641,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -57213,7 +57213,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -57221,7 +57221,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -58793,7 +58793,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -58801,7 +58801,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -60373,7 +60373,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -60381,7 +60381,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
@@ -61953,7 +61953,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -61961,7 +61961,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -63533,7 +63533,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -63541,7 +63541,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -65113,7 +65113,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -65121,7 +65121,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -66693,7 +66693,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5">
@@ -66701,7 +66701,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6">
@@ -68273,7 +68273,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -68281,7 +68281,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6">
@@ -69853,7 +69853,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
@@ -69861,7 +69861,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
@@ -71433,7 +71433,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -71441,7 +71441,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -73013,7 +73013,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -73021,7 +73021,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -74593,7 +74593,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -74601,7 +74601,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -76173,7 +76173,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -76181,7 +76181,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -77753,7 +77753,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
@@ -77761,7 +77761,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
@@ -79333,7 +79333,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
@@ -79341,7 +79341,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -80913,7 +80913,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -80921,7 +80921,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -82493,7 +82493,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -82501,7 +82501,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -84073,7 +84073,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -84081,7 +84081,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -85653,7 +85653,7 @@
         <v>44822</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -85661,7 +85661,7 @@
         <v>44821</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">

</xml_diff>